<commit_message>
New sample reduction steps
</commit_message>
<xml_diff>
--- a/Output/SAMPLE_REDUCTION_STEPS_GRADES.xlsx
+++ b/Output/SAMPLE_REDUCTION_STEPS_GRADES.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="34">
   <si>
     <t>data_prep_step</t>
   </si>
@@ -83,10 +83,16 @@
     <t>binary_nolags</t>
   </si>
   <si>
+    <t>binary_all_int_poly</t>
+  </si>
+  <si>
     <t>multi_all</t>
   </si>
   <si>
     <t>multi_nolags</t>
+  </si>
+  <si>
+    <t>multi_all_int_poly</t>
   </si>
   <si>
     <t>controls_bef_outcome</t>
@@ -222,7 +228,7 @@
       </c>
       <c r="B3"/>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D3"/>
       <c r="E3"/>
@@ -246,7 +252,7 @@
       </c>
       <c r="B4"/>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D4"/>
       <c r="E4"/>
@@ -270,7 +276,7 @@
       </c>
       <c r="B5"/>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D5"/>
       <c r="E5"/>
@@ -294,7 +300,7 @@
       </c>
       <c r="B6"/>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D6"/>
       <c r="E6"/>
@@ -318,7 +324,7 @@
       </c>
       <c r="B7"/>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D7"/>
       <c r="E7"/>
@@ -342,7 +348,7 @@
       </c>
       <c r="B8"/>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D8"/>
       <c r="E8"/>
@@ -366,7 +372,7 @@
       </c>
       <c r="B9"/>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D9"/>
       <c r="E9"/>
@@ -390,7 +396,7 @@
       </c>
       <c r="B10"/>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D10"/>
       <c r="E10"/>
@@ -414,7 +420,7 @@
       </c>
       <c r="B11"/>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D11"/>
       <c r="E11"/>
@@ -438,7 +444,7 @@
       </c>
       <c r="B12"/>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D12"/>
       <c r="E12"/>
@@ -462,7 +468,7 @@
       </c>
       <c r="B13"/>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D13"/>
       <c r="E13"/>
@@ -486,7 +492,7 @@
       </c>
       <c r="B14"/>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D14"/>
       <c r="E14"/>
@@ -510,13 +516,13 @@
       </c>
       <c r="B15"/>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E15" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
@@ -538,13 +544,13 @@
       </c>
       <c r="B16"/>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E16" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F16"/>
       <c r="G16" t="n">
@@ -566,16 +572,16 @@
       </c>
       <c r="B17"/>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F17" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G17" t="n">
         <v>6096.0</v>
@@ -596,16 +602,16 @@
       </c>
       <c r="B18"/>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E18" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F18" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G18" t="n">
         <v>3423.0</v>
@@ -626,16 +632,16 @@
       </c>
       <c r="B19"/>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D19" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E19" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F19" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G19" t="n">
         <v>6096.0</v>
@@ -656,16 +662,16 @@
       </c>
       <c r="B20"/>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D20" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E20" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F20" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G20" t="n">
         <v>3423.0</v>
@@ -688,16 +694,16 @@
         <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D21" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E21" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F21" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G21" t="n">
         <v>3423.0</v>
@@ -709,7 +715,7 @@
         <v>533.0</v>
       </c>
       <c r="J21" t="n" s="2">
-        <v>45013.55617631051</v>
+        <v>45016.53902233542</v>
       </c>
     </row>
     <row r="22">
@@ -720,16 +726,16 @@
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D22" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E22" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F22" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G22" t="n">
         <v>3423.0</v>
@@ -741,7 +747,7 @@
         <v>413.0</v>
       </c>
       <c r="J22" t="n" s="2">
-        <v>45013.55618606003</v>
+        <v>45016.53903940576</v>
       </c>
     </row>
     <row r="23">
@@ -752,16 +758,16 @@
         <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D23" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E23" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F23" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G23" t="n">
         <v>3423.0</v>
@@ -770,10 +776,10 @@
         <v>4369.0</v>
       </c>
       <c r="I23" t="n">
-        <v>537.0</v>
+        <v>41689.8</v>
       </c>
       <c r="J23" t="n" s="2">
-        <v>45013.556200987136</v>
+        <v>45016.53951428564</v>
       </c>
     </row>
     <row r="24">
@@ -784,16 +790,16 @@
         <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E24" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F24" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G24" t="n">
         <v>3423.0</v>
@@ -802,10 +808,10 @@
         <v>4369.0</v>
       </c>
       <c r="I24" t="n">
-        <v>418.0</v>
+        <v>537.0</v>
       </c>
       <c r="J24" t="n" s="2">
-        <v>45013.55621155968</v>
+        <v>45016.53954786547</v>
       </c>
     </row>
     <row r="25">
@@ -813,31 +819,31 @@
         <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D25" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F25" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G25" t="n">
-        <v>5513.0</v>
+        <v>3423.0</v>
       </c>
       <c r="H25" t="n">
-        <v>11633.0</v>
+        <v>4369.0</v>
       </c>
       <c r="I25" t="n">
-        <v>510.0</v>
+        <v>418.0</v>
       </c>
       <c r="J25" t="n" s="2">
-        <v>45013.55664447271</v>
+        <v>45016.539559743585</v>
       </c>
     </row>
     <row r="26">
@@ -845,31 +851,31 @@
         <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D26" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E26" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F26" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G26" t="n">
-        <v>5513.0</v>
+        <v>3423.0</v>
       </c>
       <c r="H26" t="n">
-        <v>11633.0</v>
+        <v>4369.0</v>
       </c>
       <c r="I26" t="n">
-        <v>422.0</v>
+        <v>41693.8</v>
       </c>
       <c r="J26" t="n" s="2">
-        <v>45013.55665386796</v>
+        <v>45016.54004558876</v>
       </c>
     </row>
     <row r="27">
@@ -877,19 +883,19 @@
         <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C27" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D27" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E27" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F27" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G27" t="n">
         <v>5513.0</v>
@@ -898,10 +904,10 @@
         <v>11633.0</v>
       </c>
       <c r="I27" t="n">
-        <v>514.0</v>
+        <v>510.0</v>
       </c>
       <c r="J27" t="n" s="2">
-        <v>45013.55667813042</v>
+        <v>45016.58160722502</v>
       </c>
     </row>
     <row r="28">
@@ -909,19 +915,19 @@
         <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C28" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D28" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E28" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F28" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G28" t="n">
         <v>5513.0</v>
@@ -930,10 +936,10 @@
         <v>11633.0</v>
       </c>
       <c r="I28" t="n">
-        <v>427.0</v>
+        <v>422.0</v>
       </c>
       <c r="J28" t="n" s="2">
-        <v>45013.55668798661</v>
+        <v>45016.58162372446</v>
       </c>
     </row>
     <row r="29">
@@ -941,31 +947,31 @@
         <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C29" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D29" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E29" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F29" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="G29" t="n">
-        <v>6096.0</v>
+        <v>5513.0</v>
       </c>
       <c r="H29" t="n">
-        <v>12918.0</v>
+        <v>11633.0</v>
       </c>
       <c r="I29" t="n">
-        <v>510.0</v>
+        <v>38275.2</v>
       </c>
       <c r="J29" t="n" s="2">
-        <v>45013.557126268584</v>
+        <v>45016.5827655724</v>
       </c>
     </row>
     <row r="30">
@@ -973,31 +979,31 @@
         <v>20</v>
       </c>
       <c r="B30" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C30" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D30" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E30" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F30" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="G30" t="n">
-        <v>6096.0</v>
+        <v>5513.0</v>
       </c>
       <c r="H30" t="n">
-        <v>12918.0</v>
+        <v>11633.0</v>
       </c>
       <c r="I30" t="n">
-        <v>422.0</v>
+        <v>514.0</v>
       </c>
       <c r="J30" t="n" s="2">
-        <v>45013.55713941001</v>
+        <v>45016.58294077299</v>
       </c>
     </row>
     <row r="31">
@@ -1005,31 +1011,31 @@
         <v>20</v>
       </c>
       <c r="B31" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C31" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D31" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E31" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F31" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="G31" t="n">
-        <v>6096.0</v>
+        <v>5513.0</v>
       </c>
       <c r="H31" t="n">
-        <v>12918.0</v>
+        <v>11633.0</v>
       </c>
       <c r="I31" t="n">
-        <v>514.0</v>
+        <v>427.0</v>
       </c>
       <c r="J31" t="n" s="2">
-        <v>45013.5571592926</v>
+        <v>45016.58295274566</v>
       </c>
     </row>
     <row r="32">
@@ -1037,31 +1043,31 @@
         <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C32" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D32" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E32" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F32" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="G32" t="n">
-        <v>6096.0</v>
+        <v>5513.0</v>
       </c>
       <c r="H32" t="n">
-        <v>12918.0</v>
+        <v>11633.0</v>
       </c>
       <c r="I32" t="n">
-        <v>427.0</v>
+        <v>38279.2</v>
       </c>
       <c r="J32" t="n" s="2">
-        <v>45013.5571684951</v>
+        <v>45016.584056991946</v>
       </c>
     </row>
     <row r="33">
@@ -1072,28 +1078,28 @@
         <v>21</v>
       </c>
       <c r="C33" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D33" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E33" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G33" t="n">
-        <v>5249.0</v>
+        <v>6096.0</v>
       </c>
       <c r="H33" t="n">
-        <v>11122.0</v>
+        <v>12918.0</v>
       </c>
       <c r="I33" t="n">
         <v>510.0</v>
       </c>
       <c r="J33" t="n" s="2">
-        <v>45013.5576153339</v>
+        <v>45016.63171210086</v>
       </c>
     </row>
     <row r="34">
@@ -1104,28 +1110,28 @@
         <v>22</v>
       </c>
       <c r="C34" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D34" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E34" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G34" t="n">
-        <v>5249.0</v>
+        <v>6096.0</v>
       </c>
       <c r="H34" t="n">
-        <v>11122.0</v>
+        <v>12918.0</v>
       </c>
       <c r="I34" t="n">
         <v>422.0</v>
       </c>
       <c r="J34" t="n" s="2">
-        <v>45013.557625513975</v>
+        <v>45016.63172652626</v>
       </c>
     </row>
     <row r="35">
@@ -1136,28 +1142,28 @@
         <v>23</v>
       </c>
       <c r="C35" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D35" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E35" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G35" t="n">
-        <v>5249.0</v>
+        <v>6096.0</v>
       </c>
       <c r="H35" t="n">
-        <v>11122.0</v>
+        <v>12918.0</v>
       </c>
       <c r="I35" t="n">
-        <v>514.0</v>
+        <v>38275.2</v>
       </c>
       <c r="J35" t="n" s="2">
-        <v>45013.55765096923</v>
+        <v>45016.63295916363</v>
       </c>
     </row>
     <row r="36">
@@ -1168,28 +1174,28 @@
         <v>24</v>
       </c>
       <c r="C36" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D36" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E36" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G36" t="n">
-        <v>5249.0</v>
+        <v>6096.0</v>
       </c>
       <c r="H36" t="n">
-        <v>11122.0</v>
+        <v>12918.0</v>
       </c>
       <c r="I36" t="n">
-        <v>427.0</v>
+        <v>514.0</v>
       </c>
       <c r="J36" t="n" s="2">
-        <v>45013.55766391179</v>
+        <v>45016.63316953114</v>
       </c>
     </row>
     <row r="37">
@@ -1197,31 +1203,31 @@
         <v>20</v>
       </c>
       <c r="B37" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C37" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D37" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E37" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G37" t="n">
-        <v>4068.0</v>
+        <v>6096.0</v>
       </c>
       <c r="H37" t="n">
-        <v>4193.0</v>
+        <v>12918.0</v>
       </c>
       <c r="I37" t="n">
-        <v>501.0</v>
+        <v>427.0</v>
       </c>
       <c r="J37" t="n" s="2">
-        <v>45013.558059790186</v>
+        <v>45016.63318411076</v>
       </c>
     </row>
     <row r="38">
@@ -1229,31 +1235,31 @@
         <v>20</v>
       </c>
       <c r="B38" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C38" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D38" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E38" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F38" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G38" t="n">
-        <v>4068.0</v>
+        <v>6096.0</v>
       </c>
       <c r="H38" t="n">
-        <v>4193.0</v>
+        <v>12918.0</v>
       </c>
       <c r="I38" t="n">
-        <v>413.0</v>
+        <v>38279.2</v>
       </c>
       <c r="J38" t="n" s="2">
-        <v>45013.55806887455</v>
+        <v>45016.63445361249</v>
       </c>
     </row>
     <row r="39">
@@ -1261,31 +1267,31 @@
         <v>20</v>
       </c>
       <c r="B39" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C39" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D39" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E39" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F39" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G39" t="n">
-        <v>4068.0</v>
+        <v>5249.0</v>
       </c>
       <c r="H39" t="n">
-        <v>4193.0</v>
+        <v>11122.0</v>
       </c>
       <c r="I39" t="n">
-        <v>506.0</v>
+        <v>510.0</v>
       </c>
       <c r="J39" t="n" s="2">
-        <v>45013.55808465592</v>
+        <v>45016.67639037313</v>
       </c>
     </row>
     <row r="40">
@@ -1293,31 +1299,351 @@
         <v>20</v>
       </c>
       <c r="B40" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" t="s">
+        <v>28</v>
+      </c>
+      <c r="D40" t="s">
+        <v>29</v>
+      </c>
+      <c r="E40" t="s">
+        <v>31</v>
+      </c>
+      <c r="F40" t="s">
+        <v>33</v>
+      </c>
+      <c r="G40" t="n">
+        <v>5249.0</v>
+      </c>
+      <c r="H40" t="n">
+        <v>11122.0</v>
+      </c>
+      <c r="I40" t="n">
+        <v>422.0</v>
+      </c>
+      <c r="J40" t="n" s="2">
+        <v>45016.676399416305</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" t="s">
+        <v>28</v>
+      </c>
+      <c r="D41" t="s">
+        <v>29</v>
+      </c>
+      <c r="E41" t="s">
+        <v>31</v>
+      </c>
+      <c r="F41" t="s">
+        <v>33</v>
+      </c>
+      <c r="G41" t="n">
+        <v>5249.0</v>
+      </c>
+      <c r="H41" t="n">
+        <v>11122.0</v>
+      </c>
+      <c r="I41" t="n">
+        <v>38275.2</v>
+      </c>
+      <c r="J41" t="n" s="2">
+        <v>45016.677207099514</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" t="s">
         <v>24</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C42" t="s">
+        <v>28</v>
+      </c>
+      <c r="D42" t="s">
+        <v>29</v>
+      </c>
+      <c r="E42" t="s">
+        <v>31</v>
+      </c>
+      <c r="F42" t="s">
+        <v>33</v>
+      </c>
+      <c r="G42" t="n">
+        <v>5249.0</v>
+      </c>
+      <c r="H42" t="n">
+        <v>11122.0</v>
+      </c>
+      <c r="I42" t="n">
+        <v>514.0</v>
+      </c>
+      <c r="J42" t="n" s="2">
+        <v>45016.67728781602</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>20</v>
+      </c>
+      <c r="B43" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" t="s">
+        <v>28</v>
+      </c>
+      <c r="D43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E43" t="s">
+        <v>31</v>
+      </c>
+      <c r="F43" t="s">
+        <v>33</v>
+      </c>
+      <c r="G43" t="n">
+        <v>5249.0</v>
+      </c>
+      <c r="H43" t="n">
+        <v>11122.0</v>
+      </c>
+      <c r="I43" t="n">
+        <v>427.0</v>
+      </c>
+      <c r="J43" t="n" s="2">
+        <v>45016.67729731133</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>20</v>
+      </c>
+      <c r="B44" t="s">
         <v>26</v>
       </c>
-      <c r="D40" t="s">
-        <v>28</v>
-      </c>
-      <c r="E40" t="s">
-        <v>29</v>
-      </c>
-      <c r="F40" t="s">
-        <v>31</v>
-      </c>
-      <c r="G40" t="n">
+      <c r="C44" t="s">
+        <v>28</v>
+      </c>
+      <c r="D44" t="s">
+        <v>29</v>
+      </c>
+      <c r="E44" t="s">
+        <v>31</v>
+      </c>
+      <c r="F44" t="s">
+        <v>33</v>
+      </c>
+      <c r="G44" t="n">
+        <v>5249.0</v>
+      </c>
+      <c r="H44" t="n">
+        <v>11122.0</v>
+      </c>
+      <c r="I44" t="n">
+        <v>38279.2</v>
+      </c>
+      <c r="J44" t="n" s="2">
+        <v>45016.67810355543</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" t="s">
+        <v>28</v>
+      </c>
+      <c r="D45" t="s">
+        <v>30</v>
+      </c>
+      <c r="E45" t="s">
+        <v>31</v>
+      </c>
+      <c r="F45" t="s">
+        <v>33</v>
+      </c>
+      <c r="G45" t="n">
         <v>4068.0</v>
       </c>
-      <c r="H40" t="n">
+      <c r="H45" t="n">
         <v>4193.0</v>
       </c>
-      <c r="I40" t="n">
+      <c r="I45" t="n">
+        <v>501.0</v>
+      </c>
+      <c r="J45" t="n" s="2">
+        <v>45016.70578025638</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>20</v>
+      </c>
+      <c r="B46" t="s">
+        <v>22</v>
+      </c>
+      <c r="C46" t="s">
+        <v>28</v>
+      </c>
+      <c r="D46" t="s">
+        <v>30</v>
+      </c>
+      <c r="E46" t="s">
+        <v>31</v>
+      </c>
+      <c r="F46" t="s">
+        <v>33</v>
+      </c>
+      <c r="G46" t="n">
+        <v>4068.0</v>
+      </c>
+      <c r="H46" t="n">
+        <v>4193.0</v>
+      </c>
+      <c r="I46" t="n">
+        <v>413.0</v>
+      </c>
+      <c r="J46" t="n" s="2">
+        <v>45016.705790383865</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>20</v>
+      </c>
+      <c r="B47" t="s">
+        <v>23</v>
+      </c>
+      <c r="C47" t="s">
+        <v>28</v>
+      </c>
+      <c r="D47" t="s">
+        <v>30</v>
+      </c>
+      <c r="E47" t="s">
+        <v>31</v>
+      </c>
+      <c r="F47" t="s">
+        <v>33</v>
+      </c>
+      <c r="G47" t="n">
+        <v>4068.0</v>
+      </c>
+      <c r="H47" t="n">
+        <v>4193.0</v>
+      </c>
+      <c r="I47" t="n">
+        <v>38012.6</v>
+      </c>
+      <c r="J47" t="n" s="2">
+        <v>45016.706116527654</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>20</v>
+      </c>
+      <c r="B48" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" t="s">
+        <v>28</v>
+      </c>
+      <c r="D48" t="s">
+        <v>30</v>
+      </c>
+      <c r="E48" t="s">
+        <v>31</v>
+      </c>
+      <c r="F48" t="s">
+        <v>33</v>
+      </c>
+      <c r="G48" t="n">
+        <v>4068.0</v>
+      </c>
+      <c r="H48" t="n">
+        <v>4193.0</v>
+      </c>
+      <c r="I48" t="n">
+        <v>506.0</v>
+      </c>
+      <c r="J48" t="n" s="2">
+        <v>45016.706141853</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>20</v>
+      </c>
+      <c r="B49" t="s">
+        <v>25</v>
+      </c>
+      <c r="C49" t="s">
+        <v>28</v>
+      </c>
+      <c r="D49" t="s">
+        <v>30</v>
+      </c>
+      <c r="E49" t="s">
+        <v>31</v>
+      </c>
+      <c r="F49" t="s">
+        <v>33</v>
+      </c>
+      <c r="G49" t="n">
+        <v>4068.0</v>
+      </c>
+      <c r="H49" t="n">
+        <v>4193.0</v>
+      </c>
+      <c r="I49" t="n">
         <v>419.0</v>
       </c>
-      <c r="J40" t="n" s="2">
-        <v>45013.55809510721</v>
+      <c r="J49" t="n" s="2">
+        <v>45016.70615089923</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>20</v>
+      </c>
+      <c r="B50" t="s">
+        <v>26</v>
+      </c>
+      <c r="C50" t="s">
+        <v>28</v>
+      </c>
+      <c r="D50" t="s">
+        <v>30</v>
+      </c>
+      <c r="E50" t="s">
+        <v>31</v>
+      </c>
+      <c r="F50" t="s">
+        <v>33</v>
+      </c>
+      <c r="G50" t="n">
+        <v>4068.0</v>
+      </c>
+      <c r="H50" t="n">
+        <v>4193.0</v>
+      </c>
+      <c r="I50" t="n">
+        <v>38017.6</v>
+      </c>
+      <c r="J50" t="n" s="2">
+        <v>45016.70647793199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>